<commit_message>
sydw Signed-off-by: fengjinliang <fengjinliang@streamhub.tech>
</commit_message>
<xml_diff>
--- a/sydw/2020上/考点/经济.xlsx
+++ b/sydw/2020上/考点/经济.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7140" activeTab="1"/>
+    <workbookView windowWidth="20175" windowHeight="11670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="社会主义市场经济体制" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="240">
   <si>
     <t>经济制度</t>
   </si>
@@ -710,6 +710,33 @@
   </si>
   <si>
     <t>容易</t>
+  </si>
+  <si>
+    <t>指吸收公众存款、发放贷款、办理结算等业务，并以利润为主要经营目标的金融机构。</t>
+  </si>
+  <si>
+    <t>1.存款业务。这个是基础业务</t>
+  </si>
+  <si>
+    <t>商业银行</t>
+  </si>
+  <si>
+    <t>主要业务有三类</t>
+  </si>
+  <si>
+    <t>2.贷款业务。这个是利润主要来源</t>
+  </si>
+  <si>
+    <t>3.结算业务</t>
+  </si>
+  <si>
+    <t>正外部性？负外部性？？？</t>
+  </si>
+  <si>
+    <t>周期性行业</t>
+  </si>
+  <si>
+    <t>外汇储备</t>
   </si>
 </sst>
 </file>
@@ -718,9 +745,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -738,8 +765,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -753,17 +789,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -771,6 +799,80 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -785,67 +887,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -860,25 +902,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -891,187 +918,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1085,49 +1112,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1148,17 +1142,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1174,6 +1168,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1182,16 +1185,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1200,133 +1227,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1669,7 +1696,7 @@
       <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="3" width="9" style="1"/>
     <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
@@ -2189,13 +2216,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C1:S70"/>
+  <dimension ref="C1:S89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="8.66666666666667" style="1"/>
     <col min="3" max="3" width="14.4166666666667" style="1" customWidth="1"/>
@@ -2392,14 +2419,12 @@
     </row>
     <row r="22" spans="3:5">
       <c r="C22" s="2"/>
-      <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="23" spans="3:5">
       <c r="C23" s="2"/>
-      <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
         <v>142</v>
       </c>
@@ -2494,7 +2519,6 @@
     <row r="34" spans="3:7">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
         <v>159</v>
       </c>
@@ -2793,6 +2817,45 @@
       </c>
       <c r="H70" s="1" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="73" spans="4:5">
+      <c r="D73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" spans="5:5">
+      <c r="E74" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5">
+      <c r="C75" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="76" spans="5:5">
+      <c r="E76" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4">
+      <c r="D88" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4">
+      <c r="D89" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2824,14 +2887,20 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="15" spans="5:5">
+      <c r="E15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>